<commit_message>
URLs Visual Comparison 1.1
</commit_message>
<xml_diff>
--- a/urls.xlsx
+++ b/urls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sabbir\Comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3F3EE0-44BB-4F6B-9AB6-E7250B29A270}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9CA8A4-DBDB-4659-BD31-B86BFA97986C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
     <t>https://www.abbviepro.com/de/de.html</t>
   </si>
   <si>
-    <t>https://www-q.abbviepro.com/de/de.html</t>
+    <t>https://dev2.abbviepro.com/de/de.html</t>
   </si>
 </sst>
 </file>
@@ -422,7 +422,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -440,24 +440,27 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{B2D6D9A6-467C-45E8-A7A2-5682F4FD3D97}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{43C45977-DA14-4E77-AEE0-79D6A3DC6751}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{138BAF19-469F-413F-939F-739222599B39}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{8CC75DF0-CD04-4A92-AC23-5B4EFF0AF4E7}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{8FAA9324-098C-49CC-AC19-36BCE886F434}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
Updated Script with readme file 2.0
</commit_message>
<xml_diff>
--- a/urls.xlsx
+++ b/urls.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sabbir\Comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9CA8A4-DBDB-4659-BD31-B86BFA97986C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB44259-953D-4218-ADF8-3D3212DAFDD7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,16 +22,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
-    <t>devUrls</t>
-  </si>
-  <si>
-    <t>prodUrls</t>
-  </si>
-  <si>
     <t>https://www.abbviepro.com/de/de.html</t>
   </si>
   <si>
     <t>https://dev2.abbviepro.com/de/de.html</t>
+  </si>
+  <si>
+    <t>testUrls</t>
+  </si>
+  <si>
+    <t>mainUrls</t>
   </si>
 </sst>
 </file>
@@ -422,7 +422,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -433,26 +433,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -463,8 +463,5 @@
     <hyperlink ref="B3" r:id="rId4" xr:uid="{8FAA9324-098C-49CC-AC19-36BCE886F434}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="A1:B1" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added captureScreenshots and compareScreenshots separately
</commit_message>
<xml_diff>
--- a/urls.xlsx
+++ b/urls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sabbir\Comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9713990-61D3-49A7-96E9-F6F2FD7E6FA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBA81A4-EAF2-4C35-ADEB-3B29E293855B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,6 +28,12 @@
     <t>mainUrls</t>
   </si>
   <si>
+    <t>https://www.abbviepro.com/de/de.html</t>
+  </si>
+  <si>
+    <t>https://www.abbviepro.com</t>
+  </si>
+  <si>
     <t>https://www.abbviepro.com/de/de/produkte/produktuebersicht.html</t>
   </si>
   <si>
@@ -35,12 +41,6 @@
   </si>
   <si>
     <t>https://www.abbviepro.com/fr/fr/neurosciences/Neurosciences/products/scyova.html</t>
-  </si>
-  <si>
-    <t>https://www.abbviepro.com/de/de.html</t>
-  </si>
-  <si>
-    <t>https://www.abbviepro.com</t>
   </si>
 </sst>
 </file>
@@ -434,7 +434,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -453,41 +453,40 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{6B47F705-C1C8-4A41-B55D-3BC668D18477}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{3D794C29-432B-4647-9C48-FEB876C38E05}"/>
-    <hyperlink ref="B2" r:id="rId3" xr:uid="{CC325D3B-6DF7-49F3-9BBE-570F528E0F3F}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{3D794C29-432B-4647-9C48-FEB876C38E05}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{CC325D3B-6DF7-49F3-9BBE-570F528E0F3F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>